<commit_message>
Adding Lab 18 HumMod data
</commit_message>
<xml_diff>
--- a/18_carbon_monoxide_inhalation/18_carbon_monoxide_inhalation_data.xlsx
+++ b/18_carbon_monoxide_inhalation/18_carbon_monoxide_inhalation_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>2000 ppm inhalation</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>Cardiac Output(mL/min)</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>The easiest way to force inspiration of CO in HumMod is to go to Lifestyle &gt; Air Supply and turn gas tanks on with 2000 PPM CO.</t>
+  </si>
+  <si>
+    <t>Patient is killed roughly 10 minutes before the 2-hour mark in HumMod. Recording data at the point of ventricular fillibration</t>
   </si>
 </sst>
 </file>
@@ -67,12 +79,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -135,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -149,11 +167,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,21 +473,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="5" t="s">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -478,9 +511,24 @@
       <c r="E2" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A3" s="6"/>
+      <c r="H2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>30</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -493,8 +541,21 @@
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="30.75" thickBot="1">
+      <c r="H3" s="7"/>
+      <c r="I3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30.75" thickBot="1">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -510,8 +571,23 @@
       <c r="E4" s="3">
         <v>42.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="45.75" thickBot="1">
+      <c r="H4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="J4" s="3">
+        <v>15.8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>30.5</v>
+      </c>
+      <c r="L4" s="3">
+        <v>49.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="45.75" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -527,8 +603,23 @@
       <c r="E5" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="45.75" thickBot="1">
+      <c r="H5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3">
+        <v>93</v>
+      </c>
+      <c r="J5" s="3">
+        <v>90</v>
+      </c>
+      <c r="K5" s="3">
+        <v>79</v>
+      </c>
+      <c r="L5" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="45.75" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -544,8 +635,23 @@
       <c r="E6" s="3">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="45.75" thickBot="1">
+      <c r="H6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.192</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="45.75" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -561,8 +667,23 @@
       <c r="E7" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="45.75" thickBot="1">
+      <c r="H7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="3">
+        <v>42</v>
+      </c>
+      <c r="J7" s="3">
+        <v>33</v>
+      </c>
+      <c r="K7" s="3">
+        <v>25</v>
+      </c>
+      <c r="L7" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="45.75" thickBot="1">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -578,8 +699,23 @@
       <c r="E8" s="3">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="75.75" thickBot="1">
+      <c r="H8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.123</v>
+      </c>
+      <c r="K8" s="3">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="L8" s="3">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="75.75" thickBot="1">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -595,10 +731,72 @@
       <c r="E9" s="3">
         <v>6493</v>
       </c>
+      <c r="H9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="3">
+        <v>5468</v>
+      </c>
+      <c r="J9" s="3">
+        <v>5704</v>
+      </c>
+      <c r="K9" s="3">
+        <v>6276</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="F11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="F14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="F11:M12"/>
+    <mergeCell ref="F14:M15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding percentage data to Lab 18
</commit_message>
<xml_diff>
--- a/18_carbon_monoxide_inhalation/18_carbon_monoxide_inhalation_data.xlsx
+++ b/18_carbon_monoxide_inhalation/18_carbon_monoxide_inhalation_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
   <si>
     <t>2000 ppm inhalation</t>
   </si>
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +77,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -150,10 +157,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -162,6 +170,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -179,11 +190,58 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -473,15 +531,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,8 +553,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:19">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -511,7 +569,7 @@
       <c r="E2" s="1">
         <v>2</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="1">
@@ -526,9 +584,24 @@
       <c r="L2" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A3" s="7"/>
+      <c r="O2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>30</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -541,7 +614,7 @@
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
@@ -554,8 +627,21 @@
       <c r="L3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="30.75" thickBot="1">
+      <c r="O3" s="8"/>
+      <c r="P3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="30.75" thickBot="1">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -586,8 +672,27 @@
       <c r="L4" s="3">
         <v>49.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="45.75" thickBot="1">
+      <c r="O4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" s="10">
+        <f>ABS((B4-I4)/B4)</f>
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="Q4" s="10">
+        <f t="shared" ref="Q4:Q9" si="0">ABS((C4-J4)/C4)</f>
+        <v>0.27419354838709681</v>
+      </c>
+      <c r="R4" s="10">
+        <f t="shared" ref="R4:R9" si="1">ABS((D4-K4)/D4)</f>
+        <v>0.2978723404255319</v>
+      </c>
+      <c r="S4" s="10">
+        <f t="shared" ref="S4:S9" si="2">ABS((E4-L4)/E4)</f>
+        <v>0.16312056737588668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="45.75" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -618,8 +723,27 @@
       <c r="L5" s="3">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="45.75" thickBot="1">
+      <c r="O5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="10">
+        <f t="shared" ref="P5:P9" si="3">ABS((B5-I5)/B5)</f>
+        <v>2.197802197802198E-2</v>
+      </c>
+      <c r="Q5" s="10">
+        <f t="shared" si="0"/>
+        <v>8.4337349397590355E-2</v>
+      </c>
+      <c r="R5" s="10">
+        <f t="shared" si="1"/>
+        <v>2.5974025974025976E-2</v>
+      </c>
+      <c r="S5" s="10">
+        <f t="shared" si="2"/>
+        <v>4.2857142857142858E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="45.75" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -650,8 +774,27 @@
       <c r="L6" s="3">
         <v>0.10199999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="45.75" thickBot="1">
+      <c r="O6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="10">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="Q6" s="10">
+        <f t="shared" si="0"/>
+        <v>9.4444444444444373E-2</v>
+      </c>
+      <c r="R6" s="10">
+        <f t="shared" si="1"/>
+        <v>0.10666666666666658</v>
+      </c>
+      <c r="S6" s="10">
+        <f t="shared" si="2"/>
+        <v>0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="45.75" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -682,8 +825,27 @@
       <c r="L7" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="45.75" thickBot="1">
+      <c r="O7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="10">
+        <f t="shared" si="3"/>
+        <v>2.4390243902439025E-2</v>
+      </c>
+      <c r="Q7" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="10">
+        <f t="shared" si="1"/>
+        <v>7.407407407407407E-2</v>
+      </c>
+      <c r="S7" s="10">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="45.75" thickBot="1">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -714,8 +876,27 @@
       <c r="L8" s="3">
         <v>6.9000000000000006E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="75.75" thickBot="1">
+      <c r="O8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="10">
+        <f t="shared" si="0"/>
+        <v>5.3846153846153891E-2</v>
+      </c>
+      <c r="R8" s="10">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999964E-2</v>
+      </c>
+      <c r="S8" s="10">
+        <f t="shared" si="2"/>
+        <v>0.13749999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="75.75" thickBot="1">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -746,58 +927,89 @@
       <c r="L9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="F11" s="8" t="s">
+      <c r="O9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="10">
+        <f t="shared" si="3"/>
+        <v>2.2820800598578377E-2</v>
+      </c>
+      <c r="Q9" s="10">
+        <f t="shared" si="0"/>
+        <v>4.3160204828090708E-2</v>
+      </c>
+      <c r="R9" s="10">
+        <f t="shared" si="1"/>
+        <v>8.0392494405233259E-2</v>
+      </c>
+      <c r="S9" s="10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="F11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="F14" s="8" t="s">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="F14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="F11:M12"/>
     <mergeCell ref="F14:M15"/>
+    <mergeCell ref="O2:O3"/>
   </mergeCells>
+  <conditionalFormatting sqref="P4:S9">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:S9">
+    <cfRule type="cellIs" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>